<commit_message>
Blogspot links & pictures added
</commit_message>
<xml_diff>
--- a/BackLinks.xlsx
+++ b/BackLinks.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="18">
   <si>
     <t>davaotourpackages.com</t>
   </si>
@@ -64,6 +64,12 @@
   </si>
   <si>
     <t>https://camiguinparadisetravels.blogspot.com/</t>
+  </si>
+  <si>
+    <t>https://surigaoparadise.blogspot.com/</t>
+  </si>
+  <si>
+    <t>https://boholtraveladventures.blogspot.com/</t>
   </si>
 </sst>
 </file>
@@ -450,7 +456,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D15"/>
+  <dimension ref="B2:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
@@ -570,6 +576,28 @@
         <v>11</v>
       </c>
     </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="https://www.google.com/webmasters/tools/external-links-domain-to-page?hl=en&amp;authuser=2&amp;siteUrl=http://realbreezedavaotours.com/&amp;bldomain=davaotourpackages.com"/>
@@ -585,9 +613,12 @@
     <hyperlink ref="C13" r:id="rId11"/>
     <hyperlink ref="C14" r:id="rId12"/>
     <hyperlink ref="C15" r:id="rId13"/>
+    <hyperlink ref="C16" r:id="rId14"/>
+    <hyperlink ref="B17" r:id="rId15"/>
+    <hyperlink ref="C17" r:id="rId16"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId14"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId17"/>
 </worksheet>
 </file>
 

</xml_diff>